<commit_message>
Added rest assured framework code
</commit_message>
<xml_diff>
--- a/restAssuredFramework/frameworkForAPITesting/Excel/testdata.xlsx
+++ b/restAssuredFramework/frameworkForAPITesting/Excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\restAssuredFramework\frameworkForAPITesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F9354-3B42-4820-9DA4-4BA1D3FCCF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC43321-DC51-4A00-8F8A-7F4D6E6D9B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="createCustomerWithValidKey" sheetId="1" r:id="rId1"/>
+    <sheet name="cxCreationValidKey" sheetId="1" r:id="rId1"/>
+    <sheet name="cxCreationInvalidKey" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -48,45 +49,9 @@
     <t>testEngineer3</t>
   </si>
   <si>
-    <t>testEngineer4</t>
-  </si>
-  <si>
-    <t>testEngineer5</t>
-  </si>
-  <si>
-    <t>testEngineer6</t>
-  </si>
-  <si>
-    <t>testEngineer7</t>
-  </si>
-  <si>
-    <t>testEngineer8</t>
-  </si>
-  <si>
-    <t>testEngineer9</t>
-  </si>
-  <si>
     <t>test3@mailinator.com</t>
   </si>
   <si>
-    <t>test4@mailinator.com</t>
-  </si>
-  <si>
-    <t>test5@mailinator.com</t>
-  </si>
-  <si>
-    <t>test6@mailinator.com</t>
-  </si>
-  <si>
-    <t>test7@mailinator.com</t>
-  </si>
-  <si>
-    <t>test8@mailinator.com</t>
-  </si>
-  <si>
-    <t>test9@mailinator.com</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -99,22 +64,10 @@
     <t>DescriptionTestEngineer3</t>
   </si>
   <si>
-    <t>DescriptionTestEngineer4</t>
-  </si>
-  <si>
-    <t>DescriptionTestEngineer5</t>
-  </si>
-  <si>
-    <t>DescriptionTestEngineer6</t>
-  </si>
-  <si>
-    <t>DescriptionTestEngineer7</t>
-  </si>
-  <si>
-    <t>DescriptionTestEngineer8</t>
-  </si>
-  <si>
-    <t>DescriptionTestEngineer9</t>
+    <t>2ndSheetDescriptionTestEngineer1</t>
+  </si>
+  <si>
+    <t>2ndSheetDescriptionTestEngineer2</t>
   </si>
 </sst>
 </file>
@@ -449,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -481,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -492,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -500,76 +453,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -578,14 +465,65 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{46E0B567-3408-4191-9968-E1E6365CB13D}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{BB67F0DD-C960-4484-A3A9-F75BEA01AE2C}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{E8E5B3D9-B6B3-4E5F-9618-BBCD47AEC86E}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{9233F2C3-9A33-4B50-9C5F-674984A569D3}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{46FD810B-23BD-40C2-BD2D-6768F139024B}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{B4FE57A2-30F7-49E6-910B-ECBB6C92DAA4}"/>
-    <hyperlink ref="B5" r:id="rId7" xr:uid="{952C4193-A910-47B0-9345-28C481789213}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{C0657D16-AEAF-41E5-8C72-C62133580F06}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{17B20277-826E-475F-B1D8-33BC0CA3556D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77AD6F-85AD-4D0C-B227-94C64C76B708}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{21202CAD-7BF1-4495-8018-8E7543951CC0}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{79862D18-5772-4DF0-BD42-5D0C70818EEE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>